<commit_message>
ANN with 4 rules / snake can eat almost everything but she turns only to left
</commit_message>
<xml_diff>
--- a/dataTest.xlsx
+++ b/dataTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="1340" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="2620" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>down</t>
   </si>
@@ -41,10 +41,16 @@
     <t>left</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>revard</t>
+    <t>same</t>
+  </si>
+  <si>
+    <t>distance to Food</t>
+  </si>
+  <si>
+    <t>distance to Wall</t>
+  </si>
+  <si>
+    <t>out</t>
   </si>
 </sst>
 </file>
@@ -359,15 +365,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,18 +390,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="L1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -401,13 +422,22 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -421,90 +451,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>180</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>120</v>
-      </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>80</v>
-      </c>
-      <c r="F5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>